<commit_message>
change spacing between ax
</commit_message>
<xml_diff>
--- a/chemical-engineering/heat-transfer/return.xlsx
+++ b/chemical-engineering/heat-transfer/return.xlsx
@@ -579,7 +579,7 @@
         <v>116</v>
       </c>
       <c r="B3" t="n">
-        <v>93.19999694824219</v>
+        <v>92.80000305175781</v>
       </c>
     </row>
     <row r="4">
@@ -587,7 +587,7 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>87.5</v>
+        <v>87.09999847412109</v>
       </c>
     </row>
     <row r="5">
@@ -595,7 +595,7 @@
         <v>109</v>
       </c>
       <c r="B5" t="n">
-        <v>86.22000122070312</v>
+        <v>85.69999694824219</v>
       </c>
     </row>
     <row r="6">
@@ -603,7 +603,7 @@
         <v>104</v>
       </c>
       <c r="B6" t="n">
-        <v>58.85000228881836</v>
+        <v>58.56666564941406</v>
       </c>
     </row>
     <row r="7">
@@ -611,7 +611,7 @@
         <v>74</v>
       </c>
       <c r="B7" t="n">
-        <v>57.90000152587891</v>
+        <v>57.59999847412109</v>
       </c>
     </row>
     <row r="8">
@@ -619,7 +619,7 @@
         <v>69</v>
       </c>
       <c r="B8" t="n">
-        <v>52.20000076293945</v>
+        <v>51.79999923706055</v>
       </c>
     </row>
     <row r="9">
@@ -627,7 +627,7 @@
         <v>65</v>
       </c>
       <c r="B9" t="n">
-        <v>51.25</v>
+        <v>50.83333206176758</v>
       </c>
     </row>
     <row r="10">
@@ -635,7 +635,7 @@
         <v>60</v>
       </c>
       <c r="B10" t="n">
-        <v>26.76666831970215</v>
+        <v>26.41666603088379</v>
       </c>
     </row>
     <row r="11">
@@ -643,7 +643,7 @@
         <v>30</v>
       </c>
       <c r="B11" t="n">
-        <v>25.70000076293945</v>
+        <v>25.39999961853027</v>
       </c>
     </row>
     <row r="12">

</xml_diff>